<commit_message>
Added info and home pages, additional tests and documentation.
</commit_message>
<xml_diff>
--- a/Burn-Down Chart.xlsx
+++ b/Burn-Down Chart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="232">
   <si>
     <t>Download/Install Eclipse, Java SDK, Eclipse App Engine plug-in and Github.</t>
   </si>
@@ -667,6 +667,51 @@
   </si>
   <si>
     <t>Lifetime Savings with different sized list than expected. Check to ensure exception is triggered.</t>
+  </si>
+  <si>
+    <t>Functional Acceptance Tests</t>
+  </si>
+  <si>
+    <t>If the panel wattage doubles, the electricity generated should also double. Any panel increases should directly correspond to power increases.</t>
+  </si>
+  <si>
+    <t>A panel angle of 45 degrees should cut estimated power generation by 25%.</t>
+  </si>
+  <si>
+    <t>A panel angle of 90 degrees should cut estimated power by 50%.</t>
+  </si>
+  <si>
+    <t>A panel angle of 22 degrees should cut estimated power by 12.2%.</t>
+  </si>
+  <si>
+    <t>A panel facing of south should cut estimated power by 30% (when compared to north placement).</t>
+  </si>
+  <si>
+    <t>A panel facing of north-east should cut estimated power by 7.5% (when compared to a north placement).</t>
+  </si>
+  <si>
+    <t>A panel facing of south-west should cut estimated power by 22.5% (when compared to a north placement).</t>
+  </si>
+  <si>
+    <t>Doubling the cost of electricity should also double the estimated savings from the solar panels.</t>
+  </si>
+  <si>
+    <t>Doubling the feed-in tariff should double the estimated money generated due to excess power.</t>
+  </si>
+  <si>
+    <t>Increasing the daily usage by 1kW should show a decline in excess power by 365.25kW per year.</t>
+  </si>
+  <si>
+    <t>Choosing Sydney instead of Brisbane should show an energy improvement by approximately 19%.</t>
+  </si>
+  <si>
+    <t>A north facing panel of 4000W placed at a 10 degree angle of elevation in Brisbane should generate a total of 90568kW of power over its lifetime.</t>
+  </si>
+  <si>
+    <t>A south facing panel of 3000W placed at a 15 degree angle of elevation in Brisbane should have an average yearly power generation of 3074kW, $400 yearly savings and prevent 6258 tonnes of tarbon emission.</t>
+  </si>
+  <si>
+    <t>An east facing panel of 1000W placed at an 80 degree angle of elevation in Sydney should have a total carbon savings of 30719 tonnes.</t>
   </si>
 </sst>
 </file>
@@ -789,7 +834,7 @@
       <charset val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -809,12 +854,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -906,6 +945,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -916,18 +961,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -957,8 +996,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="6.4830815067035544E-2"/>
-          <c:y val="2.8179971227445946E-2"/>
-          <c:w val="0.60630129341940375"/>
+          <c:y val="2.8179971227445949E-2"/>
+          <c:w val="0.60630129341940386"/>
           <c:h val="0.89915153911200429"/>
         </c:manualLayout>
       </c:layout>
@@ -1187,31 +1226,31 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="115822976"/>
-        <c:axId val="115824512"/>
+        <c:axId val="82761216"/>
+        <c:axId val="82762752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115822976"/>
+        <c:axId val="82761216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115824512"/>
+        <c:crossAx val="82762752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115824512"/>
+        <c:axId val="82762752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115822976"/>
+        <c:crossAx val="82761216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1224,7 +1263,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1552,7 +1591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="B62" sqref="B62:J62"/>
     </sheetView>
   </sheetViews>
@@ -1572,32 +1611,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="40.5" customHeight="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:13" ht="40.5" customHeight="1">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="1:13" ht="40.5" customHeight="1">
       <c r="A3" s="5" t="s">
@@ -3088,18 +3127,18 @@
       <c r="H47" s="3"/>
     </row>
     <row r="48" spans="1:11" ht="42" customHeight="1">
-      <c r="A48" s="24" t="s">
+      <c r="A48" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
-      <c r="J48" s="24"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
     </row>
     <row r="49" spans="1:11" ht="40.5" customHeight="1">
       <c r="A49" s="5" t="s">
@@ -3724,7 +3763,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1"/>
@@ -3735,11 +3774,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="28.5">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:16" ht="21.75" customHeight="1">
       <c r="A2" s="5" t="s">
@@ -4127,10 +4166,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49:B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1"/>
@@ -4140,11 +4179,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:5" ht="26.25" customHeight="1">
       <c r="A2" s="20"/>
@@ -4152,11 +4191,11 @@
       <c r="C2" s="20"/>
     </row>
     <row r="3" spans="1:5" ht="26.25" customHeight="1">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
     </row>
     <row r="4" spans="1:5" ht="21" customHeight="1">
       <c r="A4" s="5" t="s">
@@ -4890,20 +4929,20 @@
       <c r="C70" s="22"/>
     </row>
     <row r="71" spans="1:3" ht="21" customHeight="1">
-      <c r="A71" s="26" t="s">
+      <c r="A71" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="B71" s="26"/>
-      <c r="C71" s="26"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="29"/>
     </row>
     <row r="72" spans="1:3" ht="21" customHeight="1">
       <c r="A72" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B72" s="27" t="s">
+      <c r="B72" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C72" s="28" t="s">
+      <c r="C72" s="24" t="s">
         <v>100</v>
       </c>
     </row>
@@ -5133,20 +5172,20 @@
       <c r="C93" s="22"/>
     </row>
     <row r="94" spans="1:3" ht="21" customHeight="1">
-      <c r="A94" s="29" t="s">
+      <c r="A94" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="B94" s="29"/>
-      <c r="C94" s="29"/>
+      <c r="B94" s="28"/>
+      <c r="C94" s="28"/>
     </row>
     <row r="95" spans="1:3" ht="21" customHeight="1">
       <c r="A95" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B95" s="27" t="s">
+      <c r="B95" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C95" s="28" t="s">
+      <c r="C95" s="24" t="s">
         <v>100</v>
       </c>
     </row>
@@ -5242,20 +5281,20 @@
       <c r="A104" s="3"/>
     </row>
     <row r="105" spans="1:3" ht="21" customHeight="1">
-      <c r="A105" s="29" t="s">
+      <c r="A105" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="B105" s="29"/>
-      <c r="C105" s="29"/>
+      <c r="B105" s="28"/>
+      <c r="C105" s="28"/>
     </row>
     <row r="106" spans="1:3" ht="21" customHeight="1">
       <c r="A106" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B106" s="27" t="s">
+      <c r="B106" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C106" s="28" t="s">
+      <c r="C106" s="24" t="s">
         <v>100</v>
       </c>
     </row>
@@ -5441,62 +5480,224 @@
       <c r="C123" s="22"/>
     </row>
     <row r="124" spans="1:3" ht="21" customHeight="1">
-      <c r="A124" s="3"/>
-      <c r="B124" s="21"/>
-      <c r="C124" s="22"/>
+      <c r="A124" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B124" s="28"/>
+      <c r="C124" s="28"/>
     </row>
     <row r="125" spans="1:3" ht="21" customHeight="1">
-      <c r="A125" s="3"/>
-      <c r="B125" s="21"/>
-      <c r="C125" s="22"/>
-    </row>
-    <row r="126" spans="1:3" ht="21" customHeight="1">
-      <c r="A126" s="3"/>
-      <c r="B126" s="21"/>
-      <c r="C126" s="22"/>
-    </row>
-    <row r="127" spans="1:3" ht="21" customHeight="1">
-      <c r="A127" s="3"/>
-      <c r="B127" s="21"/>
-      <c r="C127" s="22"/>
-    </row>
-    <row r="128" spans="1:3" ht="21" customHeight="1">
-      <c r="A128" s="3"/>
-      <c r="B128" s="21"/>
-      <c r="C128" s="22"/>
-    </row>
-    <row r="129" spans="1:3" ht="21" customHeight="1">
-      <c r="A129" s="3"/>
-      <c r="B129" s="21"/>
-      <c r="C129" s="22"/>
-    </row>
-    <row r="130" spans="1:3" ht="21" customHeight="1">
-      <c r="A130" s="3"/>
-      <c r="B130" s="21"/>
-      <c r="C130" s="22"/>
-    </row>
-    <row r="131" spans="1:3" ht="21" customHeight="1">
-      <c r="A131" s="3"/>
-      <c r="B131" s="21"/>
-      <c r="C131" s="22"/>
-    </row>
-    <row r="132" spans="1:3" ht="21" customHeight="1">
-      <c r="A132" s="3"/>
-      <c r="B132" s="21"/>
-      <c r="C132" s="22"/>
-    </row>
-    <row r="133" spans="1:3" ht="21" customHeight="1">
-      <c r="A133" s="3"/>
-      <c r="B133" s="21"/>
-      <c r="C133" s="22"/>
-    </row>
-    <row r="134" spans="1:3" ht="21" customHeight="1">
-      <c r="A134" s="3"/>
-      <c r="B134" s="21"/>
-      <c r="C134" s="22"/>
+      <c r="A125" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B125" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C125" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="37.5" customHeight="1">
+      <c r="A126" s="3">
+        <v>1</v>
+      </c>
+      <c r="B126" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="C126" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="30" customHeight="1">
+      <c r="A127" s="3">
+        <v>2</v>
+      </c>
+      <c r="B127" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="C127" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="27.75" customHeight="1">
+      <c r="A128" s="3">
+        <v>3</v>
+      </c>
+      <c r="B128" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="C128" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="30" customHeight="1">
+      <c r="A129" s="3">
+        <v>4</v>
+      </c>
+      <c r="B129" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="C129" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="37.5" customHeight="1">
+      <c r="A130" s="3">
+        <v>5</v>
+      </c>
+      <c r="B130" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C130" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="36.75" customHeight="1">
+      <c r="A131" s="3">
+        <v>6</v>
+      </c>
+      <c r="B131" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="C131" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="42" customHeight="1">
+      <c r="A132" s="3">
+        <v>7</v>
+      </c>
+      <c r="B132" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="C132" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="33" customHeight="1">
+      <c r="A133" s="3">
+        <v>8</v>
+      </c>
+      <c r="B133" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="C133" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="35.25" customHeight="1">
+      <c r="A134" s="3">
+        <v>9</v>
+      </c>
+      <c r="B134" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="C134" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="39.75" customHeight="1">
+      <c r="A135" s="3">
+        <v>10</v>
+      </c>
+      <c r="B135" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="C135" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="36" customHeight="1">
+      <c r="A136" s="3">
+        <v>11</v>
+      </c>
+      <c r="B136" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="C136" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="41.25" customHeight="1">
+      <c r="A137" s="3">
+        <v>12</v>
+      </c>
+      <c r="B137" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="C137" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="58.5" customHeight="1">
+      <c r="A138" s="3">
+        <v>13</v>
+      </c>
+      <c r="B138" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="C138" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="38.25" customHeight="1">
+      <c r="A139" s="3">
+        <v>14</v>
+      </c>
+      <c r="B139" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="C139" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="21" customHeight="1">
+      <c r="A140" s="3"/>
+      <c r="C140" s="22"/>
+    </row>
+    <row r="141" spans="1:3" ht="21" customHeight="1">
+      <c r="A141" s="3"/>
+      <c r="C141" s="22"/>
+    </row>
+    <row r="142" spans="1:3" ht="21" customHeight="1">
+      <c r="A142" s="3"/>
+      <c r="C142" s="22"/>
+    </row>
+    <row r="143" spans="1:3" ht="21" customHeight="1">
+      <c r="A143" s="3"/>
+      <c r="C143" s="22"/>
+    </row>
+    <row r="144" spans="1:3" ht="21" customHeight="1">
+      <c r="A144" s="3"/>
+      <c r="C144" s="22"/>
+    </row>
+    <row r="145" spans="1:3" ht="21" customHeight="1">
+      <c r="A145" s="3"/>
+      <c r="C145" s="22"/>
+    </row>
+    <row r="146" spans="1:3" ht="21" customHeight="1">
+      <c r="A146" s="3"/>
+      <c r="C146" s="22"/>
+    </row>
+    <row r="147" spans="1:3" ht="21" customHeight="1">
+      <c r="A147" s="3"/>
+      <c r="C147" s="22"/>
+    </row>
+    <row r="148" spans="1:3" ht="21" customHeight="1">
+      <c r="A148" s="3"/>
+      <c r="C148" s="22"/>
+    </row>
+    <row r="149" spans="1:3" ht="21" customHeight="1">
+      <c r="A149" s="3"/>
+      <c r="C149" s="22"/>
+    </row>
+    <row r="150" spans="1:3" ht="21" customHeight="1">
+      <c r="A150" s="3"/>
+      <c r="C150" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A124:C124"/>
     <mergeCell ref="A105:C105"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A71:C71"/>

</xml_diff>